<commit_message>
1. peep sound 2. break between runs 3. easy practice trials 3. reverse phase is not quite a sucess.
</commit_message>
<xml_diff>
--- a/stairDefinitions.xlsx
+++ b/stairDefinitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yxq5055/github/sex-diffs-abramov-2012-replication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB65E33-25DB-4E48-9CD9-C1FD0625444C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42ACF77-473C-4B43-8E7F-134F70574415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26380" yWindow="7600" windowWidth="23180" windowHeight="18280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,13 +529,13 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="C2">
         <v>0.2</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="E2">
         <v>12</v>

</xml_diff>

<commit_message>
update the the startval
</commit_message>
<xml_diff>
--- a/stairDefinitions.xlsx
+++ b/stairDefinitions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yxq5055/github/sex-diffs-abramov-2012-replication/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yxq5055/Documents/github/sex-diffs-abramov-2012-replication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42ACF77-473C-4B43-8E7F-134F70574415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE603D34-32ED-D245-8763-78B90C990D22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26380" yWindow="7600" windowWidth="23180" windowHeight="18280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -472,7 +472,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,7 +529,7 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C2">
         <v>0.2</v>

</xml_diff>